<commit_message>
fetching files from /products using axios
</commit_message>
<xml_diff>
--- a/PlanningSchema.xlsx
+++ b/PlanningSchema.xlsx
@@ -47,7 +47,7 @@
     <t>Create structure</t>
   </si>
   <si>
-    <t>Create product component</t>
+    <t>Create products component</t>
   </si>
 </sst>
 </file>
@@ -101,14 +101,14 @@
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -406,12 +406,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
@@ -421,144 +421,144 @@
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
     </row>
     <row r="4" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="4"/>
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
+      <c r="A5" s="3"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="4"/>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
+      <c r="A6" s="3"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="4"/>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="4"/>
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
+      <c r="A8" s="3"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="4"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
+      <c r="A9" s="3"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="4"/>
-      <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
+      <c r="A10" s="3"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="4"/>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
+      <c r="A11" s="3"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="4"/>
-      <c r="B12" s="4"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
+      <c r="A12" s="3"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="4"/>
-      <c r="B13" s="4"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
+      <c r="A13" s="3"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="4"/>
-      <c r="B14" s="4"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
+      <c r="A14" s="3"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="4"/>
-      <c r="B15" s="4"/>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
+      <c r="A15" s="3"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="4"/>
-      <c r="B16" s="4"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="4"/>
+      <c r="A16" s="3"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="4"/>
-      <c r="B17" s="4"/>
-      <c r="C17" s="4"/>
-      <c r="D17" s="4"/>
+      <c r="A17" s="3"/>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="4"/>
-      <c r="B18" s="4"/>
-      <c r="C18" s="4"/>
-      <c r="D18" s="4"/>
+      <c r="A18" s="3"/>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="4"/>
-      <c r="B19" s="4"/>
-      <c r="C19" s="4"/>
-      <c r="D19" s="4"/>
+      <c r="A19" s="3"/>
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="4"/>
-      <c r="B20" s="4"/>
-      <c r="C20" s="4"/>
-      <c r="D20" s="4"/>
+      <c r="A20" s="3"/>
+      <c r="B20" s="3"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="4"/>
-      <c r="B21" s="4"/>
-      <c r="C21" s="4"/>
-      <c r="D21" s="4"/>
+      <c r="A21" s="3"/>
+      <c r="B21" s="3"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="4"/>
-      <c r="B22" s="4"/>
-      <c r="C22" s="4"/>
-      <c r="D22" s="4"/>
+      <c r="A22" s="3"/>
+      <c r="B22" s="3"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Creating inner class components inside the given html structure and retrieving information from API
</commit_message>
<xml_diff>
--- a/PlanningSchema.xlsx
+++ b/PlanningSchema.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
   <si>
     <t>Feature</t>
   </si>
@@ -38,9 +38,6 @@
     <t>Desired web development workflow</t>
   </si>
   <si>
-    <t>Duration</t>
-  </si>
-  <si>
     <t>Create structure for the website, using html and css elements</t>
   </si>
   <si>
@@ -48,13 +45,31 @@
   </si>
   <si>
     <t>Create products component</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>Duration - Hours</t>
+  </si>
+  <si>
+    <t>Adding new components on the given html structure is not working when importing scripts so that there will be inner react class components</t>
+  </si>
+  <si>
+    <t>Retrieving and storing information from API</t>
+  </si>
+  <si>
+    <t>Declare state inside the constructor</t>
+  </si>
+  <si>
+    <t>Progress</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -72,6 +87,14 @@
     </font>
     <font>
       <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -98,7 +121,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -109,6 +132,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -396,7 +422,7 @@
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B4" sqref="B4"/>
+      <selection pane="bottomRight" activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -420,7 +446,7 @@
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -431,32 +457,48 @@
         <v>2</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-    </row>
-    <row r="4" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+      <c r="B4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
+      <c r="D4" s="3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="5"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>

</xml_diff>